<commit_message>
Updates on tracking page and logged track page
</commit_message>
<xml_diff>
--- a/cnpjs/cnpjs.xlsx
+++ b/cnpjs/cnpjs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielcarvalho/Library/CloudStorage/GoogleDrive-gabrielkemmer@k9agency.digital/My Drive/Guilherme - App Transportadora/cnpjs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B336D9B9-E2B5-FA47-BDDC-D77BDA0AFB6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19DA20B2-9A7B-134B-A1EA-696A56956EF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="760" windowWidth="30240" windowHeight="15960" xr2:uid="{2E6ACEB9-AC91-1D41-88DF-77AB2CED3E3A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="15960" xr2:uid="{2E6ACEB9-AC91-1D41-88DF-77AB2CED3E3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="41">
   <si>
     <t>18.398.145/0001-58</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>PARCEIRO</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://g1.globo.com</t>
   </si>
 </sst>
 </file>
@@ -312,7 +318,20 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -500,20 +519,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E06FF967-764D-944B-844C-F11FEC9593E2}" name="Tabela1" displayName="Tabela1" ref="A1:K26" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A1:K26" xr:uid="{E06FF967-764D-944B-844C-F11FEC9593E2}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{DAF8467C-2069-1A43-A111-FBFF2A29C680}" name="CTE" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{A3755C34-5764-7743-86FA-AC90E2AC06D9}" name="NFE" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{3F0159BE-DDCE-0545-8DD3-8A8D5B046144}" name="DATA" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{F7DB526F-0D09-044F-A482-D11EDFAFB909}" name="CNPJ REMETENTE" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{31A5EF5E-5BCD-F542-B70D-EECA04B8A33F}" name="CLIENTE REMETENTE" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{04B011B5-8A3C-554B-8866-BEFCB3248362}" name="CLIENTE DESTINO" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{F0037241-DEFB-8744-99B0-04FA7DCA506C}" name="R$ NF" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{3FF267E9-6BA0-9245-B2F4-8F6FBA017C62}" name="PESO" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{1BD3CC0D-A5CB-7D4E-81E2-4113E612CE81}" name="QTD VOLUMES" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{9F749270-2B96-8444-B1BA-B782A7CBEBE7}" name="R$ CTE" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{AF3E426E-3997-8747-868D-6C6AFDDA4353}" name="PARCEIRO" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E06FF967-764D-944B-844C-F11FEC9593E2}" name="Tabela1" displayName="Tabela1" ref="A1:L26" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A1:L26" xr:uid="{E06FF967-764D-944B-844C-F11FEC9593E2}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{DAF8467C-2069-1A43-A111-FBFF2A29C680}" name="CTE" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{A3755C34-5764-7743-86FA-AC90E2AC06D9}" name="NFE" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{3F0159BE-DDCE-0545-8DD3-8A8D5B046144}" name="DATA" dataDxfId="9"/>
+    <tableColumn id="11" xr3:uid="{F7DB526F-0D09-044F-A482-D11EDFAFB909}" name="CNPJ REMETENTE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{31A5EF5E-5BCD-F542-B70D-EECA04B8A33F}" name="CLIENTE REMETENTE" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{04B011B5-8A3C-554B-8866-BEFCB3248362}" name="CLIENTE DESTINO" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{F0037241-DEFB-8744-99B0-04FA7DCA506C}" name="R$ NF" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{3FF267E9-6BA0-9245-B2F4-8F6FBA017C62}" name="PESO" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{1BD3CC0D-A5CB-7D4E-81E2-4113E612CE81}" name="QTD VOLUMES" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{9F749270-2B96-8444-B1BA-B782A7CBEBE7}" name="R$ CTE" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{AF3E426E-3997-8747-868D-6C6AFDDA4353}" name="PARCEIRO" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{528A606D-F4CB-AD4C-A012-18FCC5D6378C}" name="Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -816,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5A9250-C237-B840-B1F1-2D2F9C86A0D7}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="155" zoomScaleNormal="155" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -834,11 +854,11 @@
     <col min="8" max="8" width="7.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1640625" style="1"/>
+    <col min="11" max="12" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>28</v>
       </c>
@@ -872,8 +892,11 @@
       <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>43</v>
       </c>
@@ -907,8 +930,11 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A3" s="7">
         <v>44</v>
       </c>
@@ -942,8 +968,11 @@
       <c r="K3" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L3" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A4" s="3">
         <v>45</v>
       </c>
@@ -977,8 +1006,11 @@
       <c r="K4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="7">
         <v>46</v>
       </c>
@@ -1012,8 +1044,11 @@
       <c r="K5" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A6" s="3">
         <v>47</v>
       </c>
@@ -1047,8 +1082,11 @@
       <c r="K6" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L6" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A7" s="7">
         <v>48</v>
       </c>
@@ -1082,8 +1120,11 @@
       <c r="K7" s="10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A8" s="3">
         <v>49</v>
       </c>
@@ -1117,8 +1158,11 @@
       <c r="K8" s="6">
         <v>250</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A9" s="7">
         <v>50</v>
       </c>
@@ -1152,8 +1196,11 @@
       <c r="K9" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
         <v>51</v>
       </c>
@@ -1187,8 +1234,11 @@
       <c r="K10" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A11" s="7">
         <v>52</v>
       </c>
@@ -1220,8 +1270,11 @@
         <v>50</v>
       </c>
       <c r="K11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A12" s="3">
         <v>53</v>
       </c>
@@ -1255,8 +1308,11 @@
       <c r="K12" s="6">
         <v>700</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A13" s="7">
         <v>54</v>
       </c>
@@ -1290,8 +1346,11 @@
       <c r="K13" s="10">
         <v>700</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A14" s="3">
         <v>55</v>
       </c>
@@ -1325,8 +1384,11 @@
       <c r="K14" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L14" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A15" s="7">
         <v>56</v>
       </c>
@@ -1360,8 +1422,11 @@
       <c r="K15" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A16" s="3">
         <v>57</v>
       </c>
@@ -1395,8 +1460,11 @@
       <c r="K16" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A17" s="7">
         <v>58</v>
       </c>
@@ -1430,8 +1498,11 @@
       <c r="K17" s="10">
         <v>4410</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A18" s="3">
         <v>59</v>
       </c>
@@ -1465,8 +1536,11 @@
       <c r="K18" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A19" s="7">
         <v>60</v>
       </c>
@@ -1500,8 +1574,11 @@
       <c r="K19" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A20" s="3">
         <v>61</v>
       </c>
@@ -1535,8 +1612,11 @@
       <c r="K20" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L20" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A21" s="7">
         <v>62</v>
       </c>
@@ -1570,8 +1650,11 @@
       <c r="K21" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L21" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A22" s="3">
         <v>63</v>
       </c>
@@ -1605,8 +1688,11 @@
       <c r="K22" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L22" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A23" s="7">
         <v>64</v>
       </c>
@@ -1640,8 +1726,11 @@
       <c r="K23" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L23" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A24" s="3">
         <v>65</v>
       </c>
@@ -1675,8 +1764,11 @@
       <c r="K24" s="6">
         <v>3900</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A25" s="7">
         <v>66</v>
       </c>
@@ -1710,8 +1802,11 @@
       <c r="K25" s="10">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="12" x14ac:dyDescent="0.15">
+      <c r="L25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="12" x14ac:dyDescent="0.15">
       <c r="A26" s="11">
         <v>67</v>
       </c>
@@ -1744,6 +1839,9 @@
       </c>
       <c r="K26" s="14">
         <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>